<commit_message>
all the test file got parameterised. and created enhanced assertion for all test files. now assertion looks good
</commit_message>
<xml_diff>
--- a/reports/KS_tests_report.xlsx
+++ b/reports/KS_tests_report.xlsx
@@ -30,7 +30,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -41,12 +41,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00366092"/>
         <bgColor rgb="00366092"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFC7CE"/>
-        <bgColor rgb="00FFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -74,7 +68,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -86,9 +80,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -562,12 +553,12 @@
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I2" s="4" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -611,12 +602,12 @@
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I3" s="5" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -660,12 +651,12 @@
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I4" s="5" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -709,12 +700,12 @@
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I5" s="4" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -758,12 +749,12 @@
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I6" s="4" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -810,7 +801,7 @@
           <t>Ks Tests functionality verified</t>
         </is>
       </c>
-      <c r="I7" s="5" t="inlineStr">
+      <c r="I7" s="4" t="inlineStr">
         <is>
           <t>PASSED</t>
         </is>
@@ -856,12 +847,12 @@
       </c>
       <c r="H8" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I8" s="5" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -905,12 +896,12 @@
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I9" s="5" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -954,12 +945,12 @@
       </c>
       <c r="H10" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I10" s="4" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1003,12 +994,12 @@
       </c>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I11" s="5" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1025,7 +1016,7 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>Verify email required validation is visible.</t>
+          <t>Verify email required validation is visible &amp; Next button in disabled.</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
@@ -1052,12 +1043,12 @@
       </c>
       <c r="H12" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I12" s="4" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1101,12 +1092,12 @@
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I13" s="5" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1150,12 +1141,12 @@
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I14" s="4" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1199,12 +1190,12 @@
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I15" s="5" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1248,12 +1239,12 @@
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I16" s="4" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
core functional test cases of company. unsolved test cases of company details edit
</commit_message>
<xml_diff>
--- a/reports/KS_tests_report.xlsx
+++ b/reports/KS_tests_report.xlsx
@@ -30,7 +30,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -47,6 +47,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00C6EFCE"/>
         <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -68,7 +74,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -80,6 +86,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -553,12 +562,12 @@
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I2" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -602,12 +611,12 @@
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I3" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -651,12 +660,12 @@
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I4" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I4" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -700,12 +709,12 @@
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I5" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I5" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -749,12 +758,12 @@
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I6" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Test failed - actual behavior did not match expected result</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>FAILED</t>
         </is>
       </c>
     </row>
@@ -847,12 +856,12 @@
       </c>
       <c r="H8" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I8" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I8" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -896,12 +905,12 @@
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I9" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I9" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -945,12 +954,12 @@
       </c>
       <c r="H10" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I10" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Test failed - actual behavior did not match expected result</t>
+        </is>
+      </c>
+      <c r="I10" s="5" t="inlineStr">
+        <is>
+          <t>FAILED</t>
         </is>
       </c>
     </row>
@@ -994,12 +1003,12 @@
       </c>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I11" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I11" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -1043,12 +1052,12 @@
       </c>
       <c r="H12" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I12" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I12" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -1092,12 +1101,12 @@
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I13" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Test failed - actual behavior did not match expected result</t>
+        </is>
+      </c>
+      <c r="I13" s="5" t="inlineStr">
+        <is>
+          <t>FAILED</t>
         </is>
       </c>
     </row>
@@ -1141,12 +1150,12 @@
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I14" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I14" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -1190,12 +1199,12 @@
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I15" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Ks Tests functionality verified</t>
+        </is>
+      </c>
+      <c r="I15" s="4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
         </is>
       </c>
     </row>
@@ -1239,12 +1248,12 @@
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>Test not executed</t>
-        </is>
-      </c>
-      <c r="I16" s="3" t="inlineStr">
-        <is>
-          <t>Not Run</t>
+          <t>Test failed - actual behavior did not match expected result</t>
+        </is>
+      </c>
+      <c r="I16" s="5" t="inlineStr">
+        <is>
+          <t>FAILED</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
workable script for company name edit and assertion. wrote edit and assert value for other fields too but there are some issues in those scripts
</commit_message>
<xml_diff>
--- a/reports/KS_tests_report.xlsx
+++ b/reports/KS_tests_report.xlsx
@@ -30,7 +30,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -47,12 +47,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00C6EFCE"/>
         <bgColor rgb="00C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFC7CE"/>
-        <bgColor rgb="00FFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -74,7 +68,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -86,9 +80,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -758,12 +749,12 @@
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I6" s="5" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -807,12 +798,12 @@
       </c>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -856,12 +847,12 @@
       </c>
       <c r="H8" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I8" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -905,12 +896,12 @@
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I9" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -954,12 +945,12 @@
       </c>
       <c r="H10" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I10" s="5" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1003,12 +994,12 @@
       </c>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I11" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1052,12 +1043,12 @@
       </c>
       <c r="H12" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I12" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1101,12 +1092,12 @@
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I13" s="5" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1150,12 +1141,12 @@
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I14" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1199,12 +1190,12 @@
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>Ks Tests functionality verified</t>
-        </is>
-      </c>
-      <c r="I15" s="4" t="inlineStr">
-        <is>
-          <t>PASSED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>
@@ -1248,12 +1239,12 @@
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>Test failed - actual behavior did not match expected result</t>
-        </is>
-      </c>
-      <c r="I16" s="5" t="inlineStr">
-        <is>
-          <t>FAILED</t>
+          <t>Test not executed</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>Not Run</t>
         </is>
       </c>
     </row>

</xml_diff>